<commit_message>
60 data are calculated
</commit_message>
<xml_diff>
--- a/Hydrometer_V8.xlsx
+++ b/Hydrometer_V8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdnas\Desktop\ANN excel Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1BE422-0915-4B9F-B2E4-B5322C870D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A912EF-E6A0-4015-8436-7DD4A1DE6DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="30" r:id="rId1"/>
@@ -2668,14 +2668,53 @@
     <xf numFmtId="1" fontId="1" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="2" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2701,45 +2740,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="2" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8115,7 +8115,7 @@
       <sheetData sheetId="1">
         <row r="36">
           <cell r="D36">
-            <v>41</v>
+            <v>34</v>
           </cell>
         </row>
         <row r="45">
@@ -8565,18 +8565,18 @@
     </row>
     <row r="7" spans="1:37" ht="13" x14ac:dyDescent="0.25">
       <c r="J7" s="84"/>
-      <c r="K7" s="217"/>
-      <c r="L7" s="217"/>
-      <c r="M7" s="217"/>
-      <c r="N7" s="217"/>
-      <c r="O7" s="217"/>
-      <c r="P7" s="218"/>
-      <c r="Q7" s="218"/>
-      <c r="R7" s="218"/>
+      <c r="K7" s="231"/>
+      <c r="L7" s="231"/>
+      <c r="M7" s="231"/>
+      <c r="N7" s="231"/>
+      <c r="O7" s="231"/>
+      <c r="P7" s="232"/>
+      <c r="Q7" s="232"/>
+      <c r="R7" s="232"/>
       <c r="S7" s="85"/>
-      <c r="T7" s="219"/>
-      <c r="U7" s="220"/>
-      <c r="V7" s="220"/>
+      <c r="T7" s="228"/>
+      <c r="U7" s="233"/>
+      <c r="V7" s="233"/>
       <c r="AG7" s="34"/>
       <c r="AH7" s="34"/>
       <c r="AI7" s="34"/>
@@ -8587,33 +8587,33 @@
       <c r="A8" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="231" t="s">
+      <c r="B8" s="217" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="231"/>
-      <c r="D8" s="231"/>
-      <c r="E8" s="231"/>
-      <c r="F8" s="219" t="s">
+      <c r="C8" s="217"/>
+      <c r="D8" s="217"/>
+      <c r="E8" s="217"/>
+      <c r="F8" s="228" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="243" t="s">
+      <c r="G8" s="230" t="s">
         <v>144</v>
       </c>
-      <c r="H8" s="243"/>
-      <c r="I8" s="243"/>
+      <c r="H8" s="230"/>
+      <c r="I8" s="230"/>
       <c r="J8" s="84"/>
-      <c r="K8" s="217"/>
-      <c r="L8" s="217"/>
-      <c r="M8" s="217"/>
-      <c r="N8" s="217"/>
-      <c r="O8" s="217"/>
-      <c r="P8" s="218"/>
-      <c r="Q8" s="218"/>
-      <c r="R8" s="218"/>
+      <c r="K8" s="231"/>
+      <c r="L8" s="231"/>
+      <c r="M8" s="231"/>
+      <c r="N8" s="231"/>
+      <c r="O8" s="231"/>
+      <c r="P8" s="232"/>
+      <c r="Q8" s="232"/>
+      <c r="R8" s="232"/>
       <c r="S8" s="85"/>
-      <c r="T8" s="221"/>
-      <c r="U8" s="221"/>
-      <c r="V8" s="220"/>
+      <c r="T8" s="234"/>
+      <c r="U8" s="234"/>
+      <c r="V8" s="233"/>
       <c r="AG8" s="34"/>
       <c r="AH8" s="34"/>
       <c r="AI8" s="34"/>
@@ -8630,23 +8630,23 @@
       <c r="C9" s="95"/>
       <c r="D9" s="95"/>
       <c r="E9" s="95"/>
-      <c r="F9" s="219"/>
-      <c r="G9" s="243"/>
-      <c r="H9" s="243"/>
-      <c r="I9" s="243"/>
+      <c r="F9" s="228"/>
+      <c r="G9" s="230"/>
+      <c r="H9" s="230"/>
+      <c r="I9" s="230"/>
       <c r="J9" s="84"/>
-      <c r="K9" s="217"/>
-      <c r="L9" s="217"/>
-      <c r="M9" s="217"/>
-      <c r="N9" s="217"/>
-      <c r="O9" s="217"/>
-      <c r="P9" s="217"/>
-      <c r="Q9" s="217"/>
-      <c r="R9" s="217"/>
+      <c r="K9" s="231"/>
+      <c r="L9" s="231"/>
+      <c r="M9" s="231"/>
+      <c r="N9" s="231"/>
+      <c r="O9" s="231"/>
+      <c r="P9" s="231"/>
+      <c r="Q9" s="231"/>
+      <c r="R9" s="231"/>
       <c r="S9" s="85"/>
       <c r="T9" s="87"/>
-      <c r="U9" s="221"/>
-      <c r="V9" s="220"/>
+      <c r="U9" s="234"/>
+      <c r="V9" s="233"/>
       <c r="AG9" s="34"/>
       <c r="AH9" s="34"/>
       <c r="AI9" s="34"/>
@@ -8657,29 +8657,29 @@
       <c r="A10" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="231" t="s">
+      <c r="B10" s="217" t="s">
         <v>145</v>
       </c>
-      <c r="C10" s="231"/>
-      <c r="D10" s="231"/>
-      <c r="E10" s="231"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="243"/>
-      <c r="H10" s="243"/>
-      <c r="I10" s="243"/>
+      <c r="C10" s="217"/>
+      <c r="D10" s="217"/>
+      <c r="E10" s="217"/>
+      <c r="F10" s="228"/>
+      <c r="G10" s="230"/>
+      <c r="H10" s="230"/>
+      <c r="I10" s="230"/>
       <c r="J10" s="84"/>
       <c r="K10" s="96"/>
-      <c r="L10" s="225"/>
-      <c r="M10" s="225"/>
-      <c r="N10" s="225"/>
-      <c r="O10" s="225"/>
-      <c r="P10" s="225"/>
-      <c r="Q10" s="225"/>
-      <c r="R10" s="225"/>
-      <c r="S10" s="225"/>
-      <c r="T10" s="226"/>
-      <c r="U10" s="226"/>
-      <c r="V10" s="226"/>
+      <c r="L10" s="238"/>
+      <c r="M10" s="238"/>
+      <c r="N10" s="238"/>
+      <c r="O10" s="238"/>
+      <c r="P10" s="238"/>
+      <c r="Q10" s="238"/>
+      <c r="R10" s="238"/>
+      <c r="S10" s="238"/>
+      <c r="T10" s="239"/>
+      <c r="U10" s="239"/>
+      <c r="V10" s="239"/>
       <c r="AG10" s="34"/>
       <c r="AH10" s="34"/>
       <c r="AI10" s="34"/>
@@ -8696,10 +8696,10 @@
       </c>
       <c r="D11" s="91"/>
       <c r="E11" s="92"/>
-      <c r="F11" s="219"/>
-      <c r="G11" s="243"/>
-      <c r="H11" s="243"/>
-      <c r="I11" s="243"/>
+      <c r="F11" s="228"/>
+      <c r="G11" s="230"/>
+      <c r="H11" s="230"/>
+      <c r="I11" s="230"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -8767,11 +8767,11 @@
       <c r="F13" s="88" t="s">
         <v>100</v>
       </c>
-      <c r="G13" s="242" t="s">
+      <c r="G13" s="229" t="s">
         <v>154</v>
       </c>
-      <c r="H13" s="242"/>
-      <c r="I13" s="242"/>
+      <c r="H13" s="229"/>
+      <c r="I13" s="229"/>
       <c r="J13" s="79" t="s">
         <v>46</v>
       </c>
@@ -8807,9 +8807,9 @@
       </c>
       <c r="E14" s="93"/>
       <c r="F14" s="104"/>
-      <c r="G14" s="242"/>
-      <c r="H14" s="242"/>
-      <c r="I14" s="242"/>
+      <c r="G14" s="229"/>
+      <c r="H14" s="229"/>
+      <c r="I14" s="229"/>
       <c r="J14" s="20" t="s">
         <v>47</v>
       </c>
@@ -9223,18 +9223,18 @@
       </c>
       <c r="K27" s="31"/>
       <c r="L27" s="30"/>
-      <c r="M27" s="227" t="s">
+      <c r="M27" s="240" t="s">
         <v>51</v>
       </c>
-      <c r="N27" s="228"/>
+      <c r="N27" s="241"/>
       <c r="O27" s="29" t="s">
         <v>52</v>
       </c>
       <c r="P27" s="31"/>
-      <c r="Q27" s="229">
+      <c r="Q27" s="242">
         <v>867452</v>
       </c>
-      <c r="R27" s="230"/>
+      <c r="R27" s="243"/>
       <c r="S27" s="33" t="s">
         <v>55</v>
       </c>
@@ -9339,15 +9339,15 @@
         <v>53</v>
       </c>
       <c r="K30" s="31"/>
-      <c r="L30" s="222" t="s">
+      <c r="L30" s="235" t="s">
         <v>86</v>
       </c>
-      <c r="M30" s="223"/>
-      <c r="N30" s="223"/>
-      <c r="O30" s="223"/>
-      <c r="P30" s="223"/>
-      <c r="Q30" s="223"/>
-      <c r="R30" s="224"/>
+      <c r="M30" s="236"/>
+      <c r="N30" s="236"/>
+      <c r="O30" s="236"/>
+      <c r="P30" s="236"/>
+      <c r="Q30" s="236"/>
+      <c r="R30" s="237"/>
       <c r="S30" s="29" t="s">
         <v>64</v>
       </c>
@@ -9511,7 +9511,7 @@
       <c r="J35" s="174" t="s">
         <v>150</v>
       </c>
-      <c r="K35" s="232" t="s">
+      <c r="K35" s="218" t="s">
         <v>103</v>
       </c>
       <c r="L35" s="26">
@@ -9569,7 +9569,7 @@
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
       <c r="J36" s="26"/>
-      <c r="K36" s="233"/>
+      <c r="K36" s="219"/>
       <c r="L36" s="26">
         <f>'input-output'!E6</f>
         <v>0.5</v>
@@ -9625,7 +9625,7 @@
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
       <c r="J37" s="26"/>
-      <c r="K37" s="233"/>
+      <c r="K37" s="219"/>
       <c r="L37" s="26">
         <f>'input-output'!E7</f>
         <v>1</v>
@@ -9681,7 +9681,7 @@
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.25">
       <c r="J38" s="26"/>
-      <c r="K38" s="233"/>
+      <c r="K38" s="219"/>
       <c r="L38" s="26">
         <f>'input-output'!E8</f>
         <v>2</v>
@@ -9737,7 +9737,7 @@
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
       <c r="J39" s="26"/>
-      <c r="K39" s="233"/>
+      <c r="K39" s="219"/>
       <c r="L39" s="26">
         <f>'input-output'!E9</f>
         <v>4</v>
@@ -9794,7 +9794,7 @@
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40" s="82"/>
       <c r="J40" s="26"/>
-      <c r="K40" s="233"/>
+      <c r="K40" s="219"/>
       <c r="L40" s="26">
         <f>'input-output'!E10</f>
         <v>8</v>
@@ -9851,7 +9851,7 @@
     <row r="41" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A41" s="82"/>
       <c r="J41" s="26"/>
-      <c r="K41" s="233"/>
+      <c r="K41" s="219"/>
       <c r="L41" s="26">
         <f>'input-output'!E11</f>
         <v>15</v>
@@ -9909,7 +9909,7 @@
       <c r="B42" s="7"/>
       <c r="G42" s="7"/>
       <c r="J42" s="26"/>
-      <c r="K42" s="233"/>
+      <c r="K42" s="219"/>
       <c r="L42" s="26">
         <f>'input-output'!E12</f>
         <v>30</v>
@@ -9965,7 +9965,7 @@
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">
       <c r="J43" s="26"/>
-      <c r="K43" s="233"/>
+      <c r="K43" s="219"/>
       <c r="L43" s="26">
         <f>'input-output'!E13</f>
         <v>60</v>
@@ -10032,7 +10032,7 @@
         <v>89</v>
       </c>
       <c r="J44" s="26"/>
-      <c r="K44" s="233"/>
+      <c r="K44" s="219"/>
       <c r="L44" s="26">
         <f>'input-output'!E14</f>
         <v>120</v>
@@ -10088,7 +10088,7 @@
     </row>
     <row r="45" spans="1:40" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J45" s="26"/>
-      <c r="K45" s="233"/>
+      <c r="K45" s="219"/>
       <c r="L45" s="26">
         <f>'input-output'!E15</f>
         <v>240</v>
@@ -10144,7 +10144,7 @@
     </row>
     <row r="46" spans="1:40" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J46" s="26"/>
-      <c r="K46" s="233"/>
+      <c r="K46" s="219"/>
       <c r="L46" s="26">
         <f>'input-output'!E16</f>
         <v>480</v>
@@ -10210,7 +10210,7 @@
       <c r="H47" s="101"/>
       <c r="I47" s="101"/>
       <c r="J47" s="77"/>
-      <c r="K47" s="233"/>
+      <c r="K47" s="219"/>
       <c r="L47" s="26">
         <f>'input-output'!E17</f>
         <v>1434</v>
@@ -10259,7 +10259,7 @@
         <f>24*60</f>
         <v>1440</v>
       </c>
-      <c r="X47" s="235" t="s">
+      <c r="X47" s="221" t="s">
         <v>104</v>
       </c>
       <c r="AC47" s="24"/>
@@ -10283,7 +10283,7 @@
       <c r="H48" s="101"/>
       <c r="I48" s="101"/>
       <c r="J48" s="77"/>
-      <c r="K48" s="233"/>
+      <c r="K48" s="219"/>
       <c r="L48" s="26">
         <f>'input-output'!E18</f>
         <v>2865</v>
@@ -10331,7 +10331,7 @@
       <c r="W48" s="109">
         <v>2880</v>
       </c>
-      <c r="X48" s="236"/>
+      <c r="X48" s="222"/>
       <c r="AC48" s="24"/>
       <c r="AD48" s="24"/>
       <c r="AE48" s="51"/>
@@ -10353,7 +10353,7 @@
       <c r="H49" s="101"/>
       <c r="I49" s="101"/>
       <c r="J49" s="77"/>
-      <c r="K49" s="234"/>
+      <c r="K49" s="220"/>
       <c r="L49" s="26">
         <f>'input-output'!E19</f>
         <v>4306</v>
@@ -10401,7 +10401,7 @@
       <c r="W49" s="110">
         <v>4320</v>
       </c>
-      <c r="X49" s="237"/>
+      <c r="X49" s="223"/>
       <c r="AC49" s="24"/>
       <c r="AD49" s="24"/>
       <c r="AE49" s="51"/>
@@ -10843,10 +10843,10 @@
       </c>
     </row>
     <row r="75" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B75" s="238" t="s">
+      <c r="B75" s="224" t="s">
         <v>114</v>
       </c>
-      <c r="C75" s="239"/>
+      <c r="C75" s="225"/>
       <c r="J75" s="12">
         <v>24</v>
       </c>
@@ -10859,8 +10859,8 @@
       </c>
     </row>
     <row r="76" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B76" s="240"/>
-      <c r="C76" s="241"/>
+      <c r="B76" s="226"/>
+      <c r="C76" s="227"/>
       <c r="J76" s="12">
         <v>25</v>
       </c>
@@ -11688,14 +11688,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="K35:K49"/>
-    <mergeCell ref="X47:X49"/>
-    <mergeCell ref="B75:C76"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="G13:I14"/>
-    <mergeCell ref="G8:I11"/>
     <mergeCell ref="K7:R7"/>
     <mergeCell ref="T7:V7"/>
     <mergeCell ref="K8:R8"/>
@@ -11707,6 +11699,14 @@
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="K9:R9"/>
     <mergeCell ref="U9:V9"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="K35:K49"/>
+    <mergeCell ref="X47:X49"/>
+    <mergeCell ref="B75:C76"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="G13:I14"/>
+    <mergeCell ref="G8:I11"/>
   </mergeCells>
   <pageMargins left="1.1000000000000001" right="0.75" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" blackAndWhite="1" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -11729,7 +11729,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="J36" sqref="J36:P36"/>
     </sheetView>
   </sheetViews>
@@ -12569,7 +12569,7 @@
       </c>
       <c r="M36" s="216">
         <f>[1]Report!$D$36</f>
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N36" s="216">
         <f>[1]Report!$I$45</f>
@@ -12661,7 +12661,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -13160,7 +13160,7 @@
       <c r="C8" s="157"/>
       <c r="D8" s="157"/>
       <c r="E8" s="157"/>
-      <c r="F8" s="219" t="s">
+      <c r="F8" s="228" t="s">
         <v>45</v>
       </c>
       <c r="G8" s="253" t="str">
@@ -13181,7 +13181,7 @@
       <c r="C9" s="156"/>
       <c r="D9" s="156"/>
       <c r="E9" s="156"/>
-      <c r="F9" s="219"/>
+      <c r="F9" s="228"/>
       <c r="G9" s="253"/>
       <c r="H9" s="253"/>
       <c r="I9" s="253"/>
@@ -13197,7 +13197,7 @@
       <c r="C10" s="156"/>
       <c r="D10" s="156"/>
       <c r="E10" s="156"/>
-      <c r="F10" s="219"/>
+      <c r="F10" s="228"/>
       <c r="G10" s="253"/>
       <c r="H10" s="253"/>
       <c r="I10" s="253"/>
@@ -13213,7 +13213,7 @@
       </c>
       <c r="D11" s="158"/>
       <c r="E11" s="99"/>
-      <c r="F11" s="219"/>
+      <c r="F11" s="228"/>
       <c r="G11" s="253"/>
       <c r="H11" s="253"/>
       <c r="I11" s="253"/>

</xml_diff>